<commit_message>
Change of naming convention of Rsolution Listing
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_rsolution_listing.xlsx
+++ b/docs/OVW Sheets/OVWDemo_rsolution_listing.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration Dec 28\OVWMigration\docs\OVW Sheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="9732" firstSheet="26" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="en_au" sheetId="1" r:id="rId1"/>
@@ -53,7 +48,7 @@
     <sheet name="zh_cn" sheetId="39" r:id="rId39"/>
     <sheet name="ja_jp" sheetId="40" r:id="rId40"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="164">
   <si>
     <t>products</t>
   </si>
@@ -549,6 +544,12 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/JP/product/hs/ucs/solutions.html</t>
+  </si>
+  <si>
+    <t>solution-listing-Rvar1</t>
+  </si>
+  <si>
+    <t>solution-listing-Rvar2</t>
   </si>
 </sst>
 </file>
@@ -624,11 +625,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -902,7 +906,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -913,14 +917,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,6 +934,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -941,6 +948,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -951,6 +961,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -981,14 +994,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,6 +1011,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1009,6 +1025,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1019,6 +1038,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1048,50 +1070,59 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>120</v>
       </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>132</v>
       </c>
@@ -1115,14 +1146,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,6 +1163,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1143,6 +1177,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1153,6 +1190,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1182,14 +1222,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,6 +1239,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1210,6 +1253,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1220,6 +1266,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1250,14 +1299,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="72.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,6 +1316,9 @@
       <c r="B1" t="s">
         <v>119</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1277,6 +1329,9 @@
       </c>
       <c r="B2" t="s">
         <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1306,14 +1361,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1323,6 +1378,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1334,6 +1392,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1344,6 +1405,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1373,14 +1437,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1390,6 +1454,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1401,6 +1468,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1411,6 +1481,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1440,14 +1513,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1457,6 +1530,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1468,6 +1544,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1478,6 +1557,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1507,14 +1589,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,6 +1606,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1535,6 +1620,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1545,6 +1633,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1574,14 +1665,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,6 +1682,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1602,6 +1696,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1612,6 +1709,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1640,13 +1740,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1656,6 +1758,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1667,6 +1772,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1677,6 +1785,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1706,14 +1817,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,6 +1834,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1734,6 +1848,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1744,6 +1861,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1773,14 +1893,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,6 +1910,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1801,6 +1924,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1811,6 +1937,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1840,14 +1969,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="73.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,6 +1986,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1868,6 +2000,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1878,6 +2013,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1907,14 +2045,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,6 +2062,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1935,6 +2076,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1945,6 +2089,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1974,14 +2121,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1991,6 +2138,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2002,6 +2152,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2012,6 +2165,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2041,14 +2197,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,6 +2214,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2069,6 +2228,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2079,6 +2241,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2108,14 +2273,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,6 +2290,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2136,6 +2304,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2146,6 +2317,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2175,14 +2349,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2192,6 +2366,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2203,6 +2380,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2213,6 +2393,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2242,14 +2425,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,6 +2442,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2270,6 +2456,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2280,6 +2469,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2309,14 +2501,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2326,6 +2518,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2337,6 +2532,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2347,6 +2545,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2376,14 +2577,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2393,6 +2594,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2404,6 +2608,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2414,6 +2621,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2443,14 +2653,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2460,6 +2670,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2471,6 +2684,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2481,6 +2697,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2510,14 +2729,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2527,6 +2746,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2538,6 +2760,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2548,6 +2773,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2577,14 +2805,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2594,6 +2822,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2605,6 +2836,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2615,6 +2849,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2644,14 +2881,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2661,6 +2898,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2672,6 +2912,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2682,6 +2925,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2711,14 +2957,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,6 +2974,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2739,6 +2988,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2749,6 +3001,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2778,14 +3033,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2795,6 +3050,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2806,6 +3064,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2816,6 +3077,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2845,14 +3109,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:A4"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2862,6 +3126,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2873,6 +3140,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2883,6 +3153,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2912,14 +3185,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2929,6 +3202,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -2940,6 +3216,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2950,6 +3229,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2979,14 +3261,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2996,6 +3278,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3007,6 +3292,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3017,6 +3305,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3046,14 +3337,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3063,6 +3354,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3074,6 +3368,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3084,6 +3381,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3113,14 +3413,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3130,6 +3430,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3141,6 +3444,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3151,6 +3457,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3179,15 +3488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3197,6 +3506,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3208,6 +3520,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3218,6 +3533,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3246,15 +3564,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,6 +3582,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3275,6 +3596,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3285,6 +3609,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3314,14 +3641,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3331,6 +3658,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3342,6 +3672,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3352,6 +3685,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3381,14 +3717,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3398,6 +3734,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3409,6 +3748,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3419,6 +3761,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3448,14 +3793,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,6 +3810,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3476,6 +3824,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3486,6 +3837,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3515,14 +3869,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,6 +3886,9 @@
       <c r="B1" t="s">
         <v>118</v>
       </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -3543,6 +3900,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3553,6 +3913,9 @@
       </c>
       <c r="B3" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>

</xml_diff>